<commit_message>
3-Excel Charts Tutorial File
</commit_message>
<xml_diff>
--- a/Excel Charts Tutorial File.xlsx
+++ b/Excel Charts Tutorial File.xlsx
@@ -1,24 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/579481080490e445/Documents/Excel Series Excels/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA04C7DD-8BCF-4FE5-B548-55CBD210AC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{03CEABDE-3C67-4836-9FDD-609F2D7E7F08}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="3" r:id="rId1"/>
     <sheet name="Chart Sheet" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>January</t>
   </si>
@@ -102,12 +96,15 @@
   <si>
     <t>Dunder Mifflin Sales Report</t>
   </si>
+  <si>
+    <t>Mois/Items</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +171,2181 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="fr-FR"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Paper</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$B$2:$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>November</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>December</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Year End Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$B$3:$N$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>485</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>736</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Printer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$B$2:$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>November</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>December</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Year End Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$B$4:$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Manila Folder</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$B$2:$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>November</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>December</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Year End Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$B$5:$N$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1583</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Staplers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$B$2:$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>November</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>December</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Year End Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$B$6:$N$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>271</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3 Ring Binder</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$B$2:$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>November</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>December</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Year End Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$B$7:$N$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>811</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Highlighters</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$B$2:$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>November</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>December</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Year End Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$B$8:$N$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>451</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$B$2:$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>November</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>December</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Year End Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$B$9:$N$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>223</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Items Per Month</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$B$2:$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>November</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>December</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Year End Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$B$10:$N$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>898</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>547</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1113</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>571</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>871</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>888</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>678</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>987</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>442</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>776</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9077</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="fr-FR"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20467432195975502"/>
+          <c:y val="0.17581036745406825"/>
+          <c:w val="0.45284711286089241"/>
+          <c:h val="0.75474518810148727"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Printer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$B$2:$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>November</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>December</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Year End Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$B$4:$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="fr-FR"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:view3D>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Paper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Printer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manila Folder</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Staplers</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3 Ring Binder</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Highlighters</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Pens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>February </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Paper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Printer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manila Folder</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Staplers</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3 Ring Binder</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Highlighters</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Pens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$C$3:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>March</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Paper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Printer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manila Folder</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Staplers</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3 Ring Binder</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Highlighters</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Pens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$D$3:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>April</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Paper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Printer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manila Folder</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Staplers</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3 Ring Binder</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Highlighters</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Pens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$E$3:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>May</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Paper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Printer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manila Folder</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Staplers</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3 Ring Binder</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Highlighters</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Pens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$F$3:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>June</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Paper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Printer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manila Folder</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Staplers</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3 Ring Binder</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Highlighters</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Pens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$G$3:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>485</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>July</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Paper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Printer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manila Folder</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Staplers</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3 Ring Binder</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Highlighters</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Pens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$H$3:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>August</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Paper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Printer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manila Folder</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Staplers</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3 Ring Binder</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Highlighters</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Pens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$I$3:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>September</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Paper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Printer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manila Folder</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Staplers</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3 Ring Binder</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Highlighters</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Pens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$J$3:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>736</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>October</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Paper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Printer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manila Folder</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Staplers</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3 Ring Binder</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Highlighters</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Pens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$K$3:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>November</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Paper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Printer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manila Folder</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Staplers</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3 Ring Binder</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Highlighters</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Pens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$L$3:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sales!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>December</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sales!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Paper</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Printer</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manila Folder</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Staplers</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3 Ring Binder</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Highlighters</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Pens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sales!$M$3:$M$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="fr-FR"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:axId val="42883712"/>
+        <c:axId val="42893696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="42883712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="42893696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="42893696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="42883712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -217,7 +2389,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -269,7 +2441,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -463,27 +2635,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41930B34-5114-49CB-81BC-662EB848F545}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -501,7 +2673,10 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -542,7 +2717,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -587,7 +2762,7 @@
         <v>5071</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -632,7 +2807,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -677,7 +2852,7 @@
         <v>1583</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -722,7 +2897,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -767,7 +2942,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -812,7 +2987,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -857,7 +3032,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -920,19 +3095,21 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B444C6-5638-496B-93B2-259D582C3A1D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>